<commit_message>
Отчет по Chekin rating score
</commit_message>
<xml_diff>
--- a/src/UntappdViewer.Reporting/Resources/StatisticsTemplate.xlsx
+++ b/src/UntappdViewer.Reporting/Resources/StatisticsTemplate.xlsx
@@ -5,16 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\Test\Untappd\UntappdViewer\src\UntappdViewer.Reporting\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{496F3A5A-100E-4DEB-B53A-E28A4ED1E19A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A7FB12-9D92-4E63-9B1C-9F4F7F5BBC13}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{46C7F45F-BA3B-49A1-9C07-4BFFCFC12068}"/>
+    <workbookView xWindow="-25320" yWindow="2430" windowWidth="25440" windowHeight="15390" xr2:uid="{46C7F45F-BA3B-49A1-9C07-4BFFCFC12068}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="1" r:id="rId1"/>
+    <sheet name="BeerChekinRatingScore" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="BeerAverageRating">BeerChekinRatingScore!$B$52</definedName>
+    <definedName name="ChekinAverageRating">BeerChekinRatingScore!$B$53</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,9 +34,29 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Rating Score</t>
+  </si>
+  <si>
+    <t>Beer Count</t>
+  </si>
+  <si>
+    <t>Chekin Count</t>
+  </si>
+  <si>
+    <t>Beer</t>
+  </si>
+  <si>
+    <t>Chekin</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -40,16 +65,31 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -57,12 +97,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -78,6 +136,1033 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Chekin rating score</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BeerChekinRatingScore!$C$52</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Beer [ average rating: ]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="6350">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:alpha val="70000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BeerChekinRatingScore!$A$2:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BeerChekinRatingScore!$B$2:$B$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-65D0-467F-9D50-B7D459BB9821}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BeerChekinRatingScore!$C$53</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Chekin [ average rating: ]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="6350">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:alpha val="70000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BeerChekinRatingScore!$A$2:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BeerChekinRatingScore!$C$2:$C$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-65D0-467F-9D50-B7D459BB9821}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1720408543"/>
+        <c:axId val="1551418959"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1720408543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1551418959"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1551418959"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1720408543"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19467907420663327"/>
+          <c:y val="0.87983034729354481"/>
+          <c:w val="0.61219585314073499"/>
+          <c:h val="8.1522309711286087E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0E1EA28-D40D-43E3-947D-389071A1C4F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,10 +1464,308 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E13F76-DCAB-4CCE-90F1-6BA6BEFE082F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.70866141732283472" bottom="0.70866141732283472" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E9F3F9-4747-45BD-A2F5-5E0795F59F74}">
+  <dimension ref="A1:C53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+    </row>
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" t="str">
+        <f>CONCATENATE(A52," [ average rating: ",B52,"]")</f>
+        <v>Beer [ average rating: ]</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" t="str">
+        <f>CONCATENATE(A53," [ average rating: ",B53,"]")</f>
+        <v>Chekin [ average rating: ]</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>